<commit_message>
Update Ibrahim Hegazi's Work Report.xlsx
</commit_message>
<xml_diff>
--- a/Work Reports/Ibrahim Hegazi's Work Report.xlsx
+++ b/Work Reports/Ibrahim Hegazi's Work Report.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\CyberSentinel-AI-Powered-Home-and-Office-Network-Security-Scanner\Work Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ibrahim_Hegazi\Desktop\MalWatch\Work Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6146018D-51B7-4CBE-8860-C645F3ABAF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C8A3FC4-C701-4B0E-8A3E-E64B5345015E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>

</xml_diff>